<commit_message>
COR-647 form changes from SC
</commit_message>
<xml_diff>
--- a/web/static/nrc_grf_template.xlsx
+++ b/web/static/nrc_grf_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">birth_date</t>
   </si>
   <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
     <t xml:space="preserve">is_minor</t>
   </si>
   <si>
@@ -103,10 +106,22 @@
     <t xml:space="preserve">preferred_communication_language</t>
   </si>
   <si>
-    <t xml:space="preserve">phone_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">phone_number_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone_number_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone_number_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email_3</t>
   </si>
   <si>
     <t xml:space="preserve">address</t>
@@ -167,6 +182,24 @@
   </si>
   <si>
     <t xml:space="preserve">identification_context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments</t>
   </si>
   <si>
     <t xml:space="preserve">collection_agent_name</t>
@@ -363,157 +396,157 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BN2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BD1" activeCellId="0" sqref="BD1"/>
+      <selection pane="topLeft" activeCell="BH2" activeCellId="0" sqref="BH2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="0" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="0" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="0" t="s">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="AW1" s="1" t="s">
@@ -522,7 +555,7 @@
       <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="0" t="s">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="AZ1" s="1" t="s">
@@ -537,142 +570,200 @@
       <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="2" t="b">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>32051</v>
       </c>
-      <c r="G2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="0" t="n">
+      <c r="G2" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="S2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="U2" s="2" t="b">
+      <c r="V2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="2" t="b">
+      <c r="W2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AH2" s="2" t="b">
+      <c r="AM2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AI2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AX2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AY2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AZ2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="BA2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="BB2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC2" s="0" t="s">
-        <v>75</v>
+      <c r="AN2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AS2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AU2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AY2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="BA2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AC2" r:id="rId1" display="john@email.com"/>
+    <hyperlink ref="AF2" r:id="rId1" display="john@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
COR-647 sc individual form changes (#89)
* COR-570 new individual list options
* COR-573 encode individual list options to URL (#92)
* COR-573 encode individual list options to URL
* COR-572 parse new individual list options (#93)
* COR-523 sorting (#96)

Co-authored-by: Irena Lämmerer <internetti@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/web/static/nrc_grf_template.xlsx
+++ b/web/static/nrc_grf_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">birth_date</t>
   </si>
   <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
     <t xml:space="preserve">is_minor</t>
   </si>
   <si>
@@ -103,10 +106,22 @@
     <t xml:space="preserve">preferred_communication_language</t>
   </si>
   <si>
-    <t xml:space="preserve">phone_number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">phone_number_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone_number_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone_number_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email_3</t>
   </si>
   <si>
     <t xml:space="preserve">address</t>
@@ -167,6 +182,24 @@
   </si>
   <si>
     <t xml:space="preserve">identification_context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_field_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments</t>
   </si>
   <si>
     <t xml:space="preserve">collection_agent_name</t>
@@ -363,157 +396,157 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC2"/>
+  <dimension ref="A1:BN2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BD1" activeCellId="0" sqref="BD1"/>
+      <selection pane="topLeft" activeCell="BH2" activeCellId="0" sqref="BH2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="0" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="0" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="0" t="s">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="AW1" s="1" t="s">
@@ -522,7 +555,7 @@
       <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="0" t="s">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
       <c r="AZ1" s="1" t="s">
@@ -537,142 +570,200 @@
       <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="BD1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="2" t="b">
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4" t="n">
         <v>32051</v>
       </c>
-      <c r="G2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="0" t="n">
+      <c r="G2" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="S2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="U2" s="2" t="b">
+      <c r="V2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="W2" s="2"/>
-      <c r="X2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="2" t="b">
+      <c r="W2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AH2" s="2" t="b">
+      <c r="AM2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AI2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AX2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AY2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AZ2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="BA2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="BB2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC2" s="0" t="s">
-        <v>75</v>
+      <c r="AN2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AS2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AU2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AW2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AY2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="BA2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BK2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AC2" r:id="rId1" display="john@email.com"/>
+    <hyperlink ref="AF2" r:id="rId1" display="john@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>